<commit_message>
ALMOST FINISH BUT NO CIGAR
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0-windows/Math2_Quiz.xlsx
+++ b/bin/Debug/net8.0-windows/Math2_Quiz.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>Question</t>
   </si>
@@ -140,19 +140,13 @@
     <t>What is 1/8 as a decimal?</t>
   </si>
   <si>
-    <t>What is the mean of 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11?</t>
-  </si>
-  <si>
-    <t>What is the median of 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5?</t>
-  </si>
-  <si>
-    <t>What is the mode of 2</t>
+    <t xml:space="preserve"> What is the mean of the set {0, 5, 10}?</t>
+  </si>
+  <si>
+    <t>What is the mean of the set {3, 3, 3, 3, 3, 0, 6}?</t>
+  </si>
+  <si>
+    <t>: What is the mode of the set {2, 3, 3, 5, 7}?</t>
   </si>
   <si>
     <t>What is 3² + 4²?</t>
@@ -1329,13 +1323,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="44.2222222222222" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1817,102 +1814,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
+        <v>2.5</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
-      </c>
-      <c r="G25">
-        <v>9</v>
-      </c>
-      <c r="H25">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="B26">
+        <v>1.5</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
         <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26">
-        <v>9</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26">
-        <v>4</v>
-      </c>
-      <c r="G26">
-        <v>5</v>
-      </c>
-      <c r="H26">
-        <v>7</v>
-      </c>
-      <c r="I26">
-        <v>9</v>
-      </c>
-      <c r="J26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <v>4</v>
-      </c>
-      <c r="I27">
         <v>5</v>
       </c>
-      <c r="J27" t="s">
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -1932,7 +1896,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>10</v>
@@ -1952,7 +1916,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>120</v>
@@ -1972,19 +1936,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
         <v>45</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>46</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>47</v>
-      </c>
-      <c r="D31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" t="s">
-        <v>49</v>
       </c>
       <c r="F31" t="s">
         <v>2</v>

</xml_diff>